<commit_message>
HCAP-1233 | added useful error messages and data cleanup on failure to seed-data. Test now runs and passes! But the test runner doesn't run seed-data
</commit_message>
<xml_diff>
--- a/server/scripts/xlsx/cohort_participants.xlsx
+++ b/server/scripts/xlsx/cohort_participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taraepp/Dev/hcap_workspace/hcap/server/scripts/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2EB76B-E26E-5740-A010-8E1A74000F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB6B1E2-D753-2E41-8BFB-95F6138688BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46600" yWindow="2400" windowWidth="20740" windowHeight="12280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14740" yWindow="2660" windowWidth="20740" windowHeight="12280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -442,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>

</xml_diff>